<commit_message>
add files class power bi
</commit_message>
<xml_diff>
--- a/documents/vendas.xlsx
+++ b/documents/vendas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/40cbc61c02823304/Área de Trabalho/Emanuel/Data-Analyst-Course/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{8C9D1601-1C42-492B-8189-65F9FF6145A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18E8EF1D-6BDC-4429-B700-9BB0572399E9}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{8C9D1601-1C42-492B-8189-65F9FF6145A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEF4C9E6-3D36-45AC-B178-AD2D01102925}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4A2BF8E4-2334-4FFE-84EB-0DA785503482}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{4A2BF8E4-2334-4FFE-84EB-0DA785503482}"/>
   </bookViews>
   <sheets>
     <sheet name="fVenda" sheetId="1" r:id="rId1"/>
@@ -114,13 +114,13 @@
     <t>Ar Condicionado Split Samsung Digital Inverter 8 Polos 12000 BTUs Q/F 220V</t>
   </si>
   <si>
-    <t>https://images.samsung.com/is/image/samsung/br-digital-inverter-frio-8-polos-ar12mvspbgmnaz-frontpmgray-79179982?$L2-Thumbnail$</t>
+    <t>Total Venda(R$)</t>
   </si>
   <si>
-    <t>https://www.startpage.com/av/proxy-image?piurl=https%3A%2F%2Fexitocol.vtexassets.com%2Farquivos%2Fids%2F4820320%2Fcelular-xiaomi-redmi-9-64gb-4ram-purpura-forro.jpg%3Fv%3D637396219644470000&amp;sp=1704037197T5c2eb52f32e6d3b2c46731d4840301b0444dcfcd67111715b7af2e8ee374a88e</t>
+    <t>https://www.startpage.com/av/proxy-image?piurl=https%3A%2F%2Fpurepng.com%2Fpublic%2Fuploads%2Flarge%2Fpurepng.com-samsung-phonesmartphoneandroidgooglephoneapplication-211519339028ghq1u.png&amp;sp=1704129903Ta0107b568efefd779f0a6be6f0a8f19c59d030277d0ca1b04466fd24caaf8660</t>
   </si>
   <si>
-    <t>Total Venda(R$)</t>
+    <t>https://www.startpage.com/av/proxy-image?piurl=https%3A%2F%2Fimagensemoldes.com.br%2Fwp-content%2Fuploads%2F2020%2F06%2FImagem-Ar-Condicionado-PNG.png&amp;sp=1704130110T848005e0fbcf14b79b7586f03c0173bddb4a1795d8a80f5bd97a5f4ad21cc7ad</t>
   </si>
 </sst>
 </file>
@@ -601,7 +601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6DC3264-F7B2-413E-BF9C-B8D8361CE0EC}">
   <dimension ref="A1:I1581"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -637,7 +637,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H1" t="s">
         <v>6</v>
@@ -48058,8 +48058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B159950A-3191-4AA8-ADDD-42421E08F244}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -48110,13 +48110,13 @@
         <v>23</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{75F454A0-0E5B-470E-BA9D-0A60FFBF84B1}"/>
-    <hyperlink ref="C3" r:id="rId2" display="https://www.startpage.com/av/proxy-image?piurl=https%3A%2F%2Fexitocol.vtexassets.com%2Farquivos%2Fids%2F4820320%2Fcelular-xiaomi-redmi-9-64gb-4ram-purpura-forro.jpg%3Fv%3D637396219644470000&amp;sp=1704037197T5c2eb52f32e6d3b2c46731d4840301b0444dcfcd67111715b7af2e8ee374a88e" xr:uid="{AA7B56C0-2014-48D1-94E8-67A4AFC3B034}"/>
+    <hyperlink ref="C3" r:id="rId2" display="https://www.startpage.com/av/proxy-image?piurl=https%3A%2F%2Fpurepng.com%2Fpublic%2Fuploads%2Flarge%2Fpurepng.com-samsung-phonesmartphoneandroidgooglephoneapplication-211519339028ghq1u.png&amp;sp=1704129903Ta0107b568efefd779f0a6be6f0a8f19c59d030277d0ca1b04466fd24caaf8660" xr:uid="{AA7B56C0-2014-48D1-94E8-67A4AFC3B034}"/>
     <hyperlink ref="C4" r:id="rId3" xr:uid="{1865163D-8FE5-4DE8-B439-2DEEB7F30D79}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>